<commit_message>
Fini pour de vrai
</commit_message>
<xml_diff>
--- a/Dave.xlsx
+++ b/Dave.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="17715" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="17715" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Données" sheetId="1" r:id="rId1"/>
     <sheet name="Parties contre l'IA optimale" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="29">
   <si>
     <t>Victoires</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Totaux contre l'IA à 50</t>
   </si>
   <si>
-    <t>Totaux des victoires contre les 3 IA (6,000,000 de parties jouées)</t>
-  </si>
-  <si>
     <t>Partie</t>
   </si>
   <si>
@@ -96,6 +93,15 @@
   </si>
   <si>
     <t>Nulles: 1</t>
+  </si>
+  <si>
+    <t>Totaux contre l'IA à 65</t>
+  </si>
+  <si>
+    <t>Totaux contre l'IA à 80</t>
+  </si>
+  <si>
+    <t>Totaux des victoires contre les 3 IA (270,000,000 de parties jouées)</t>
   </si>
 </sst>
 </file>
@@ -155,7 +161,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -338,11 +344,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="214739968"/>
-        <c:axId val="240567808"/>
+        <c:axId val="123726080"/>
+        <c:axId val="134992640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="214739968"/>
+        <c:axId val="123726080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -422,10 +428,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240567808"/>
+        <c:crossAx val="134992640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -433,7 +439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240567808"/>
+        <c:axId val="134992640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,10 +523,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214739968"/>
+        <c:crossAx val="123726080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -558,7 +564,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -572,7 +578,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -788,21 +794,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140868992"/>
-        <c:axId val="140878976"/>
+        <c:axId val="134895488"/>
+        <c:axId val="134901760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140868992"/>
+        <c:axId val="134895488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Diffuculté de l'IA</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140878976"/>
+        <c:crossAx val="134901760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -810,18 +835,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140878976"/>
+        <c:axId val="134901760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Nombre de parties gagnées</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140868992"/>
+        <c:crossAx val="134895488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -846,7 +890,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1058,21 +1102,45 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="151022592"/>
-        <c:axId val="151024384"/>
+        <c:axId val="136053888"/>
+        <c:axId val="136055808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="151022592"/>
+        <c:axId val="136053888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Difficulté</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CA" baseline="0"/>
+                  <a:t> de l'IA</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151024384"/>
+        <c:crossAx val="136055808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1080,18 +1148,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151024384"/>
+        <c:axId val="136055808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Noimbre de parties gagnées</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151022592"/>
+        <c:crossAx val="136053888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1116,7 +1203,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1328,21 +1415,43 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="151433216"/>
-        <c:axId val="151434752"/>
+        <c:axId val="136102272"/>
+        <c:axId val="136104192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="151433216"/>
+        <c:axId val="136102272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Diffuculté de l'IA</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151434752"/>
+        <c:crossAx val="136104192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1350,18 +1459,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151434752"/>
+        <c:axId val="136104192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Nombre de parties gagnées</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151433216"/>
+        <c:crossAx val="136102272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1973,10 +2101,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>149225</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>99482</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4667250" cy="2771775"/>
     <xdr:sp macro="" textlink="">
@@ -1986,7 +2114,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16640175" y="5962649"/>
+          <a:off x="17759892" y="6004982"/>
           <a:ext cx="4667250" cy="2771775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2092,15 +2220,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>169333</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>87842</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2709333</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>78317</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2121,16 +2249,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>115359</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2762250</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2151,16 +2279,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139701</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>1685924</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2730500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2182,15 +2310,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>229659</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>62441</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>1085850</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2199,8 +2327,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22726650" y="1819275"/>
-          <a:ext cx="8020050" cy="466725"/>
+          <a:off x="22877992" y="62441"/>
+          <a:ext cx="5189008" cy="921809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2231,7 +2359,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
           <a:r>
@@ -2244,11 +2372,112 @@
             <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
               <a:latin typeface="+mn-lt"/>
             </a:rPr>
-            <a:t> concernant le nombre de victoires selon qui joue en premier</a:t>
+            <a:t> concernant le nombre de victoires</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t> selon qui joue en premier</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:latin typeface="+mn-lt"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>124883</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>149226</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>973666</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>116418</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="ZoneTexte 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28562300" y="3197226"/>
+          <a:ext cx="5484283" cy="2824692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Analyse des parties</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Pour</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> commencer, j'ai fait douze partie avec ce que j'ai déterminé étant la meilleur intelligence artificielle. Sur les douze parties, j'ai commencer en premier pour six d'entre elles.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Je m'en suis sorti gagnant pour une seule raison, moi j'étais capable de déterminer que par exemple j'avais 20 et que l'IA avait 19, donc que j'allait gagner. Étant le premier à joue je passe mon tour, l'IA aussi a passé son tour puisqu'elle ne se base que sur les probabilités (À moins que j'aie 21), la chose que j'aurais fait (et que j'ai fait dans certaines parties) à sa place serait de jouer. En appliquant ces techinques j'ai pu m'en sortir avec plus de victoires que l'IA.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Évidemment ceci n'est pas représentatif, mais je pense quand même que je pourrais continuer à la battre, à moins qu'elle ne se mette à appliquer mes techniques.</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2646,33 +2875,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:CY39"/>
   <sheetViews>
-    <sheetView topLeftCell="O16" workbookViewId="0">
-      <selection activeCell="AB33" sqref="AB33"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
     <col min="14" max="14" width="23.85546875" customWidth="1"/>
     <col min="15" max="15" width="25.5703125" customWidth="1"/>
     <col min="16" max="16" width="26" customWidth="1"/>
     <col min="17" max="17" width="4.7109375" customWidth="1"/>
-    <col min="18" max="18" width="25.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" customWidth="1"/>
     <col min="19" max="19" width="26" customWidth="1"/>
-    <col min="20" max="20" width="17.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" customWidth="1"/>
     <col min="21" max="21" width="19" customWidth="1"/>
     <col min="22" max="22" width="19.42578125" customWidth="1"/>
     <col min="23" max="23" width="23.85546875" customWidth="1"/>
-    <col min="24" max="24" width="25.5703125" customWidth="1"/>
+    <col min="24" max="24" width="43.7109375" customWidth="1"/>
     <col min="25" max="25" width="26" customWidth="1"/>
-    <col min="26" max="26" width="23.85546875" customWidth="1"/>
-    <col min="27" max="27" width="25.5703125" customWidth="1"/>
-    <col min="28" max="28" width="26" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" customWidth="1"/>
+    <col min="27" max="27" width="13.28515625" customWidth="1"/>
+    <col min="28" max="28" width="17.7109375" customWidth="1"/>
     <col min="29" max="29" width="17.28515625" customWidth="1"/>
     <col min="30" max="30" width="19" customWidth="1"/>
     <col min="31" max="31" width="19.42578125" customWidth="1"/>
@@ -2761,7 +2992,19 @@
         <v>14</v>
       </c>
       <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
         <v>15</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:103" x14ac:dyDescent="0.25">
@@ -2813,6 +3056,18 @@
       <c r="U2" t="s">
         <v>2</v>
       </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA2">
+        <v>17</v>
+      </c>
+      <c r="AB2">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -2863,6 +3118,18 @@
       <c r="U3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA3">
+        <v>21</v>
+      </c>
+      <c r="AB3">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -2919,6 +3186,18 @@
         <f t="shared" si="1"/>
         <v>452559</v>
       </c>
+      <c r="Y4">
+        <v>3</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA4">
+        <v>16</v>
+      </c>
+      <c r="AB4">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -2975,6 +3254,18 @@
         <f t="shared" si="1"/>
         <v>508093</v>
       </c>
+      <c r="Y5">
+        <v>4</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA5">
+        <v>23</v>
+      </c>
+      <c r="AB5">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -3031,6 +3322,18 @@
         <f t="shared" si="1"/>
         <v>523132</v>
       </c>
+      <c r="Y6">
+        <v>5</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA6">
+        <v>23</v>
+      </c>
+      <c r="AB6">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -3087,6 +3390,18 @@
         <f t="shared" si="1"/>
         <v>538195</v>
       </c>
+      <c r="Y7">
+        <v>6</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA7">
+        <v>19</v>
+      </c>
+      <c r="AB7">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -3143,6 +3458,18 @@
         <f t="shared" si="1"/>
         <v>539745</v>
       </c>
+      <c r="Y8">
+        <v>7</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA8">
+        <v>20</v>
+      </c>
+      <c r="AB8">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -3199,6 +3526,18 @@
         <f t="shared" si="1"/>
         <v>538778</v>
       </c>
+      <c r="Y9">
+        <v>8</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA9">
+        <v>17</v>
+      </c>
+      <c r="AB9">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -3255,6 +3594,18 @@
         <f t="shared" si="1"/>
         <v>516029</v>
       </c>
+      <c r="Y10">
+        <v>9</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA10">
+        <v>27</v>
+      </c>
+      <c r="AB10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -3311,6 +3662,18 @@
         <f t="shared" si="1"/>
         <v>506987</v>
       </c>
+      <c r="Y11">
+        <v>10</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA11">
+        <v>12</v>
+      </c>
+      <c r="AB11">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="2:103" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -3371,19 +3734,18 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="2"/>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2"/>
-      <c r="AI12" s="2"/>
-      <c r="AJ12" s="2"/>
-      <c r="AK12" s="2"/>
+      <c r="Y12">
+        <v>11</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA12">
+        <v>21</v>
+      </c>
+      <c r="AB12">
+        <v>20</v>
+      </c>
       <c r="AL12" s="2"/>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
@@ -3464,19 +3826,18 @@
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="2"/>
-      <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="2"/>
+      <c r="Y13">
+        <v>12</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA13">
+        <v>20</v>
+      </c>
+      <c r="AB13">
+        <v>17</v>
+      </c>
       <c r="AL13" s="2"/>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
@@ -3552,7 +3913,7 @@
         <v>12</v>
       </c>
       <c r="M14" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -3565,19 +3926,6 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="2"/>
-      <c r="AH14" s="2"/>
-      <c r="AI14" s="2"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
@@ -3690,19 +4038,18 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="2"/>
-      <c r="AH15" s="2"/>
-      <c r="AI15" s="2"/>
-      <c r="AJ15" s="2"/>
-      <c r="AK15" s="2"/>
+      <c r="Y15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>25</v>
+      </c>
       <c r="AL15" s="2"/>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
@@ -3815,19 +4162,6 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="2"/>
-      <c r="AG16" s="2"/>
-      <c r="AH16" s="2"/>
-      <c r="AI16" s="2"/>
-      <c r="AJ16" s="2"/>
-      <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
@@ -3943,19 +4277,6 @@
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="2"/>
-      <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
@@ -4071,19 +4392,6 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="2"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
-      <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
@@ -4199,19 +4507,6 @@
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="2"/>
-      <c r="AD19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="2"/>
-      <c r="AG19" s="2"/>
-      <c r="AH19" s="2"/>
-      <c r="AI19" s="2"/>
-      <c r="AJ19" s="2"/>
-      <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
@@ -4327,19 +4622,6 @@
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
-      <c r="AH20" s="2"/>
-      <c r="AI20" s="2"/>
-      <c r="AJ20" s="2"/>
-      <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
@@ -4794,7 +5076,7 @@
         <v>13</v>
       </c>
       <c r="M27" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:103" x14ac:dyDescent="0.25">
@@ -5267,8 +5549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="A1:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5278,16 +5560,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5295,7 +5577,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>17</v>
@@ -5309,7 +5591,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>21</v>
@@ -5323,7 +5605,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -5337,7 +5619,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>23</v>
@@ -5351,7 +5633,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>23</v>
@@ -5365,7 +5647,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>19</v>
@@ -5379,7 +5661,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -5393,7 +5675,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>17</v>
@@ -5407,7 +5689,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>27</v>
@@ -5421,7 +5703,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -5435,7 +5717,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>21</v>
@@ -5449,7 +5731,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -5460,16 +5742,16 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>